<commit_message>
Sending Emails from stack
</commit_message>
<xml_diff>
--- a/MailMergeTasks/Book1.xlsx
+++ b/MailMergeTasks/Book1.xlsx
@@ -24,17 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Amanda</t>
   </si>
   <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello </t>
-  </si>
-  <si>
     <t>firstName</t>
   </si>
   <si>
@@ -47,30 +41,9 @@
     <t>McCarty</t>
   </si>
   <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Its..Me</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Cena</t>
-  </si>
-  <si>
     <t>amccart8@emich.edu</t>
   </si>
   <si>
-    <t>toaster727@hotmail.com</t>
-  </si>
-  <si>
-    <t>amandamc72@hotmail.com</t>
-  </si>
-  <si>
-    <t>amadnamc727@gmail.com</t>
-  </si>
-  <si>
     <t>address</t>
   </si>
   <si>
@@ -114,6 +87,51 @@
   </si>
   <si>
     <t>favColor</t>
+  </si>
+  <si>
+    <t>Geoffrey</t>
+  </si>
+  <si>
+    <t>Duong</t>
+  </si>
+  <si>
+    <t>Christine</t>
+  </si>
+  <si>
+    <t>Gallarin</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Torices</t>
+  </si>
+  <si>
+    <t>Mahmood</t>
+  </si>
+  <si>
+    <t>Zaman</t>
+  </si>
+  <si>
+    <t>gduong@emich.edu</t>
+  </si>
+  <si>
+    <t>fmahmood@emich.edu</t>
+  </si>
+  <si>
+    <t>cgallari@emich.edu</t>
+  </si>
+  <si>
+    <t>ctorices@emich.edu</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>7856 Main St</t>
   </si>
 </sst>
 </file>
@@ -451,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,112 +486,135 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>